<commit_message>
cambios varios, creacion de script para informes por pais, borrado de excel que no uso
</commit_message>
<xml_diff>
--- a/excels/niveles_unificados1.3.xlsx
+++ b/excels/niveles_unificados1.3.xlsx
@@ -5,19 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gpavez\Desktop\Compensaciones\git\compensaciones\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gpavez\Desktop\Compensaciones\git\compensaciones\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23055" windowHeight="10455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23055" windowHeight="10455" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Niveles_Unificados" sheetId="1" r:id="rId1"/>
     <sheet name="Resumen_Niveles_Por_Cargo" sheetId="2" r:id="rId2"/>
-    <sheet name="Rangos_Carlos" sheetId="3" r:id="rId3"/>
+    <sheet name="Rangos_Carlos" sheetId="3" state="hidden" r:id="rId3"/>
     <sheet name="Rangos_Deborah" sheetId="4" r:id="rId4"/>
     <sheet name="Rangos_Combinados" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Resumen_Niveles_Por_Cargo!$A$1:$D$158</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -4099,12 +4102,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -4134,11 +4143,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4443,7 +4454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H575"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A259" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18360,16 +18371,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:D158"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A158" sqref="A158"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -18386,266 +18400,275 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>848</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>1307</v>
+        <v>1336</v>
       </c>
       <c r="D2" t="s">
-        <v>1308</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>14</v>
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>1309</v>
+        <v>1323</v>
       </c>
       <c r="D3" t="s">
-        <v>1309</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>17</v>
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>1309</v>
+        <v>1321</v>
       </c>
       <c r="D4" t="s">
-        <v>1309</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>21</v>
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>1310</v>
+        <v>1330</v>
       </c>
       <c r="D5" t="s">
-        <v>1311</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>24</v>
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>888</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>1312</v>
+        <v>1332</v>
       </c>
       <c r="D6" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>962</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1309</v>
+      </c>
+      <c r="D7" t="s">
         <v>1313</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1314</v>
-      </c>
-      <c r="D7" t="s">
-        <v>1315</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>40</v>
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>903</v>
       </c>
       <c r="B8" t="s">
         <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>1310</v>
+        <v>1336</v>
       </c>
       <c r="D8" t="s">
-        <v>1316</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>45</v>
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>613</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>1317</v>
+        <v>1341</v>
       </c>
       <c r="D9" t="s">
-        <v>1307</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>53</v>
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>396</v>
       </c>
       <c r="B10" t="s">
         <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>1307</v>
+        <v>1336</v>
       </c>
       <c r="D10" t="s">
-        <v>1308</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>58</v>
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>1318</v>
+        <v>1320</v>
       </c>
       <c r="D11" t="s">
-        <v>1307</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>65</v>
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>469</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>1319</v>
+        <v>1334</v>
       </c>
       <c r="D12" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1325</v>
+      </c>
+      <c r="D13" t="s">
         <v>1313</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>72</v>
-      </c>
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" t="s">
-        <v>1307</v>
-      </c>
-      <c r="D13" t="s">
-        <v>1308</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>75</v>
+    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>883</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>1320</v>
+        <v>1336</v>
       </c>
       <c r="D14" t="s">
-        <v>1310</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>78</v>
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>841</v>
       </c>
       <c r="B15" t="s">
         <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>1321</v>
+        <v>1332</v>
       </c>
       <c r="D15" t="s">
         <v>1310</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>83</v>
+    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>371</v>
       </c>
       <c r="B16" t="s">
         <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>1319</v>
+        <v>1339</v>
       </c>
       <c r="D16" t="s">
-        <v>1322</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>88</v>
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>909</v>
       </c>
       <c r="B17" t="s">
         <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>1323</v>
+        <v>1330</v>
       </c>
       <c r="D17" t="s">
-        <v>1311</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>91</v>
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>553</v>
       </c>
       <c r="B18" t="s">
         <v>39</v>
       </c>
       <c r="C18" t="s">
+        <v>1319</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>959</v>
+      </c>
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1332</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
         <v>1323</v>
       </c>
-      <c r="D18" t="s">
-        <v>1313</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>94</v>
-      </c>
-      <c r="B19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" t="s">
-        <v>1324</v>
-      </c>
-      <c r="D19" t="s">
-        <v>1313</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>98</v>
-      </c>
-      <c r="B20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" t="s">
-        <v>1325</v>
-      </c>
       <c r="D20" t="s">
-        <v>1313</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>107</v>
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>897</v>
       </c>
       <c r="C21" t="s">
         <v>1309</v>
@@ -18654,258 +18677,258 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>112</v>
+    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>917</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
       </c>
       <c r="C22" t="s">
-        <v>1309</v>
+        <v>1336</v>
       </c>
       <c r="D22" t="s">
-        <v>1309</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>117</v>
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>1326</v>
+        <v>1319</v>
       </c>
       <c r="D23" t="s">
-        <v>1322</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>124</v>
-      </c>
-      <c r="B24" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="C24" t="s">
+        <v>1318</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" t="s">
         <v>1319</v>
       </c>
-      <c r="D24" t="s">
-        <v>1313</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>129</v>
-      </c>
-      <c r="B25" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25" t="s">
-        <v>1327</v>
-      </c>
       <c r="D25" t="s">
-        <v>1308</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>132</v>
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>755</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C26" t="s">
-        <v>1319</v>
+        <v>1321</v>
       </c>
       <c r="D26" t="s">
-        <v>1322</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>136</v>
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>239</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="C27" t="s">
-        <v>1328</v>
+        <v>1321</v>
       </c>
       <c r="D27" t="s">
-        <v>1322</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>151</v>
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>231</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>1327</v>
+        <v>1334</v>
       </c>
       <c r="D28" t="s">
-        <v>1308</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>155</v>
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>1329</v>
+        <v>1320</v>
       </c>
       <c r="D29" t="s">
-        <v>1311</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>158</v>
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>987</v>
       </c>
       <c r="B30" t="s">
         <v>39</v>
       </c>
       <c r="C30" t="s">
-        <v>1330</v>
+        <v>1321</v>
       </c>
       <c r="D30" t="s">
-        <v>1313</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>163</v>
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>701</v>
       </c>
       <c r="B31" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="C31" t="s">
+        <v>1321</v>
+      </c>
+      <c r="D31" t="s">
         <v>1310</v>
       </c>
-      <c r="D31" t="s">
-        <v>1316</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>168</v>
+    </row>
+    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>1145</v>
       </c>
       <c r="B32" t="s">
         <v>27</v>
       </c>
       <c r="C32" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="D32" t="s">
-        <v>1313</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>171</v>
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="B33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1317</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>679</v>
+      </c>
+      <c r="B34" t="s">
         <v>39</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>1319</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D34" t="s">
         <v>1310</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>826</v>
+      </c>
+      <c r="B35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1309</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B34" t="s">
-        <v>27</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="B36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" t="s">
         <v>1331</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D36" t="s">
         <v>1307</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>180</v>
-      </c>
-      <c r="B35" t="s">
-        <v>27</v>
-      </c>
-      <c r="C35" t="s">
-        <v>1332</v>
-      </c>
-      <c r="D35" t="s">
-        <v>1322</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>183</v>
-      </c>
-      <c r="B36" t="s">
-        <v>27</v>
-      </c>
-      <c r="C36" t="s">
-        <v>1325</v>
-      </c>
-      <c r="D36" t="s">
-        <v>1311</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>188</v>
+    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>248</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C37" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="D37" t="s">
-        <v>1322</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>191</v>
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>259</v>
       </c>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C38" t="s">
-        <v>1323</v>
+        <v>1319</v>
       </c>
       <c r="D38" t="s">
-        <v>1322</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>194</v>
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="B39" t="s">
         <v>39</v>
       </c>
       <c r="C39" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
       <c r="D39" t="s">
-        <v>1311</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>204</v>
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>666</v>
       </c>
       <c r="B40" t="s">
         <v>39</v>
@@ -18914,762 +18937,735 @@
         <v>1323</v>
       </c>
       <c r="D40" t="s">
-        <v>1311</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>211</v>
+      <c r="A41" s="2" t="s">
+        <v>482</v>
       </c>
       <c r="B41" t="s">
         <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>1310</v>
+        <v>1325</v>
       </c>
       <c r="D41" t="s">
-        <v>1316</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>214</v>
+      <c r="A42" s="2" t="s">
+        <v>1091</v>
       </c>
       <c r="B42" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="C42" t="s">
-        <v>1319</v>
+        <v>1307</v>
       </c>
       <c r="D42" t="s">
-        <v>1310</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>217</v>
+      <c r="A43" s="2" t="s">
+        <v>389</v>
       </c>
       <c r="B43" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C43" t="s">
-        <v>1319</v>
+        <v>1340</v>
       </c>
       <c r="D43" t="s">
-        <v>1311</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>220</v>
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>272</v>
       </c>
       <c r="B44" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="C44" t="s">
-        <v>1333</v>
+        <v>1309</v>
       </c>
       <c r="D44" t="s">
         <v>1322</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>225</v>
+        <v>1228</v>
       </c>
       <c r="B45" t="s">
-        <v>39</v>
+        <v>673</v>
       </c>
       <c r="C45" t="s">
-        <v>1327</v>
+        <v>1310</v>
       </c>
       <c r="D45" t="s">
         <v>1308</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>228</v>
+    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>774</v>
+      </c>
+      <c r="B46" t="s">
+        <v>20</v>
       </c>
       <c r="C46" t="s">
+        <v>1332</v>
+      </c>
+      <c r="D46" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B47" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1328</v>
+      </c>
+      <c r="D47" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="B48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1321</v>
+      </c>
+      <c r="D48" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B49" t="s">
+        <v>39</v>
+      </c>
+      <c r="C49" t="s">
+        <v>1323</v>
+      </c>
+      <c r="D49" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="B50" t="s">
+        <v>39</v>
+      </c>
+      <c r="C50" t="s">
         <v>1309</v>
       </c>
-      <c r="D46" t="s">
-        <v>1309</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>231</v>
-      </c>
-      <c r="B47" t="s">
-        <v>39</v>
-      </c>
-      <c r="C47" t="s">
-        <v>1334</v>
-      </c>
-      <c r="D47" t="s">
+      <c r="D50" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B51" t="s">
+        <v>27</v>
+      </c>
+      <c r="C51" t="s">
+        <v>1321</v>
+      </c>
+      <c r="D51" t="s">
         <v>1310</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>236</v>
-      </c>
-      <c r="B48" t="s">
-        <v>20</v>
-      </c>
-      <c r="C48" t="s">
-        <v>1335</v>
-      </c>
-      <c r="D48" t="s">
+    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>730</v>
+      </c>
+      <c r="B52" t="s">
+        <v>27</v>
+      </c>
+      <c r="C52" t="s">
+        <v>1336</v>
+      </c>
+      <c r="D52" t="s">
         <v>1313</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>239</v>
-      </c>
-      <c r="B49" t="s">
-        <v>27</v>
-      </c>
-      <c r="C49" t="s">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="B53" t="s">
+        <v>27</v>
+      </c>
+      <c r="C53" t="s">
         <v>1321</v>
       </c>
-      <c r="D49" t="s">
-        <v>1310</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>248</v>
-      </c>
-      <c r="B50" t="s">
-        <v>27</v>
-      </c>
-      <c r="C50" t="s">
-        <v>1321</v>
-      </c>
-      <c r="D50" t="s">
-        <v>1327</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>253</v>
-      </c>
-      <c r="B51" t="s">
-        <v>27</v>
-      </c>
-      <c r="C51" t="s">
-        <v>1307</v>
-      </c>
-      <c r="D51" t="s">
-        <v>1308</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>256</v>
-      </c>
-      <c r="B52" t="s">
-        <v>27</v>
-      </c>
-      <c r="C52" t="s">
-        <v>1320</v>
-      </c>
-      <c r="D52" t="s">
-        <v>1310</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>259</v>
-      </c>
-      <c r="B53" t="s">
-        <v>27</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>870</v>
+      </c>
+      <c r="B54" t="s">
+        <v>27</v>
+      </c>
+      <c r="C54" t="s">
         <v>1319</v>
-      </c>
-      <c r="D53" t="s">
-        <v>1327</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>262</v>
-      </c>
-      <c r="B54" t="s">
-        <v>39</v>
-      </c>
-      <c r="C54" t="s">
-        <v>1323</v>
       </c>
       <c r="D54" t="s">
         <v>1313</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>267</v>
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="B55" t="s">
         <v>27</v>
       </c>
       <c r="C55" t="s">
-        <v>1310</v>
+        <v>1332</v>
       </c>
       <c r="D55" t="s">
-        <v>1316</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>272</v>
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>549</v>
       </c>
       <c r="B56" t="s">
         <v>27</v>
       </c>
       <c r="C56" t="s">
-        <v>1309</v>
+        <v>1321</v>
       </c>
       <c r="D56" t="s">
         <v>1322</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>275</v>
+    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>412</v>
       </c>
       <c r="B57" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="C57" t="s">
-        <v>1307</v>
+        <v>1321</v>
       </c>
       <c r="D57" t="s">
-        <v>1308</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>280</v>
+      <c r="A58" s="2" t="s">
+        <v>236</v>
       </c>
       <c r="B58" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C58" t="s">
-        <v>1323</v>
+        <v>1335</v>
       </c>
       <c r="D58" t="s">
         <v>1313</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>284</v>
+    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>295</v>
       </c>
       <c r="B59" t="s">
+        <v>27</v>
+      </c>
+      <c r="C59" t="s">
+        <v>1336</v>
+      </c>
+      <c r="D59" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="B60" t="s">
         <v>10</v>
       </c>
-      <c r="C59" t="s">
-        <v>1310</v>
-      </c>
-      <c r="D59" t="s">
-        <v>1316</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>292</v>
-      </c>
-      <c r="B60" t="s">
-        <v>27</v>
-      </c>
       <c r="C60" t="s">
-        <v>1336</v>
+        <v>1319</v>
       </c>
       <c r="D60" t="s">
         <v>1313</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>295</v>
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="B61" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C61" t="s">
+        <v>1324</v>
+      </c>
+      <c r="D61" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B62" t="s">
+        <v>10</v>
+      </c>
+      <c r="C62" t="s">
+        <v>1323</v>
+      </c>
+      <c r="D62" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>984</v>
+      </c>
+      <c r="B63" t="s">
+        <v>20</v>
+      </c>
+      <c r="C63" t="s">
         <v>1336</v>
       </c>
-      <c r="D61" t="s">
-        <v>1322</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>298</v>
-      </c>
-      <c r="B62" t="s">
-        <v>39</v>
-      </c>
-      <c r="C62" t="s">
+      <c r="D63" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B64" t="s">
+        <v>27</v>
+      </c>
+      <c r="C64" t="s">
+        <v>1336</v>
+      </c>
+      <c r="D64" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>769</v>
+      </c>
+      <c r="B65" t="s">
+        <v>20</v>
+      </c>
+      <c r="C65" t="s">
+        <v>1336</v>
+      </c>
+      <c r="D65" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="B66" t="s">
+        <v>27</v>
+      </c>
+      <c r="C66" t="s">
+        <v>1330</v>
+      </c>
+      <c r="D66" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B67" t="s">
+        <v>20</v>
+      </c>
+      <c r="C67" t="s">
         <v>1325</v>
       </c>
-      <c r="D62" t="s">
-        <v>1311</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>301</v>
-      </c>
-      <c r="B63" t="s">
-        <v>27</v>
-      </c>
-      <c r="C63" t="s">
-        <v>1325</v>
-      </c>
-      <c r="D63" t="s">
-        <v>1308</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>317</v>
-      </c>
-      <c r="C64" t="s">
-        <v>1309</v>
-      </c>
-      <c r="D64" t="s">
-        <v>1309</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>322</v>
-      </c>
-      <c r="B65" t="s">
-        <v>39</v>
-      </c>
-      <c r="C65" t="s">
-        <v>1325</v>
-      </c>
-      <c r="D65" t="s">
-        <v>1308</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>331</v>
-      </c>
-      <c r="B66" t="s">
+      <c r="D67" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="B68" t="s">
+        <v>20</v>
+      </c>
+      <c r="C68" t="s">
+        <v>1336</v>
+      </c>
+      <c r="D68" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="B69" t="s">
         <v>10</v>
       </c>
-      <c r="C66" t="s">
-        <v>1307</v>
-      </c>
-      <c r="D66" t="s">
-        <v>1308</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>337</v>
-      </c>
-      <c r="B67" t="s">
-        <v>27</v>
-      </c>
-      <c r="C67" t="s">
-        <v>1337</v>
-      </c>
-      <c r="D67" t="s">
-        <v>1307</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>343</v>
-      </c>
-      <c r="B68" t="s">
-        <v>27</v>
-      </c>
-      <c r="C68" t="s">
-        <v>1338</v>
-      </c>
-      <c r="D68" t="s">
-        <v>1322</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>348</v>
-      </c>
-      <c r="B69" t="s">
-        <v>39</v>
-      </c>
       <c r="C69" t="s">
-        <v>1325</v>
+        <v>1330</v>
       </c>
       <c r="D69" t="s">
-        <v>1308</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>361</v>
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>628</v>
       </c>
       <c r="B70" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="C70" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="D70" t="s">
-        <v>1316</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>364</v>
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>854</v>
       </c>
       <c r="B71" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C71" t="s">
-        <v>1330</v>
+        <v>1319</v>
       </c>
       <c r="D71" t="s">
         <v>1313</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>371</v>
+    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>833</v>
       </c>
       <c r="B72" t="s">
         <v>27</v>
       </c>
       <c r="C72" t="s">
-        <v>1339</v>
+        <v>1330</v>
       </c>
       <c r="D72" t="s">
         <v>1313</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>378</v>
+    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>220</v>
       </c>
       <c r="B73" t="s">
         <v>10</v>
       </c>
       <c r="C73" t="s">
-        <v>1319</v>
+        <v>1333</v>
       </c>
       <c r="D73" t="s">
-        <v>1313</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>389</v>
-      </c>
-      <c r="B74" t="s">
-        <v>20</v>
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C74" t="s">
-        <v>1340</v>
+        <v>1309</v>
       </c>
       <c r="D74" t="s">
-        <v>1313</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>396</v>
-      </c>
-      <c r="B75" t="s">
-        <v>39</v>
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C75" t="s">
-        <v>1336</v>
+        <v>1309</v>
       </c>
       <c r="D75" t="s">
-        <v>1322</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>401</v>
-      </c>
-      <c r="B76" t="s">
-        <v>27</v>
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>1241</v>
       </c>
       <c r="C76" t="s">
-        <v>1325</v>
+        <v>1309</v>
       </c>
       <c r="D76" t="s">
-        <v>1311</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>412</v>
-      </c>
-      <c r="B77" t="s">
-        <v>27</v>
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>1256</v>
       </c>
       <c r="C77" t="s">
-        <v>1321</v>
+        <v>1309</v>
       </c>
       <c r="D77" t="s">
-        <v>1322</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>421</v>
-      </c>
-      <c r="B78" t="s">
-        <v>10</v>
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>228</v>
       </c>
       <c r="C78" t="s">
-        <v>1330</v>
+        <v>1309</v>
       </c>
       <c r="D78" t="s">
-        <v>1313</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>424</v>
-      </c>
-      <c r="B79" t="s">
-        <v>39</v>
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>1225</v>
       </c>
       <c r="C79" t="s">
         <v>1309</v>
       </c>
       <c r="D79" t="s">
-        <v>1322</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>436</v>
-      </c>
-      <c r="B80" t="s">
-        <v>27</v>
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="C80" t="s">
-        <v>1323</v>
+        <v>1309</v>
       </c>
       <c r="D80" t="s">
-        <v>1311</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>447</v>
-      </c>
-      <c r="B81" t="s">
-        <v>27</v>
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>1268</v>
       </c>
       <c r="C81" t="s">
-        <v>1334</v>
+        <v>1309</v>
       </c>
       <c r="D81" t="s">
-        <v>1310</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>462</v>
-      </c>
-      <c r="B82" t="s">
-        <v>39</v>
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="C82" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="D82" t="s">
-        <v>1316</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>469</v>
+        <v>1259</v>
       </c>
       <c r="B83" t="s">
         <v>39</v>
       </c>
       <c r="C83" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D83" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>1263</v>
+      </c>
+      <c r="C84" t="s">
+        <v>1309</v>
+      </c>
+      <c r="D84" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>941</v>
+      </c>
+      <c r="B85" t="s">
+        <v>20</v>
+      </c>
+      <c r="C85" t="s">
+        <v>1321</v>
+      </c>
+      <c r="D85" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>863</v>
+      </c>
+      <c r="B86" t="s">
+        <v>20</v>
+      </c>
+      <c r="C86" t="s">
+        <v>1319</v>
+      </c>
+      <c r="D86" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>912</v>
+      </c>
+      <c r="B87" t="s">
+        <v>20</v>
+      </c>
+      <c r="C87" t="s">
+        <v>1323</v>
+      </c>
+      <c r="D87" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B88" t="s">
+        <v>27</v>
+      </c>
+      <c r="C88" t="s">
+        <v>1319</v>
+      </c>
+      <c r="D88" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="C89" t="s">
+        <v>1309</v>
+      </c>
+      <c r="D89" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
+        <v>690</v>
+      </c>
+      <c r="B90" t="s">
+        <v>27</v>
+      </c>
+      <c r="C90" t="s">
+        <v>1319</v>
+      </c>
+      <c r="D90" t="s">
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B91" t="s">
+        <v>27</v>
+      </c>
+      <c r="C91" t="s">
+        <v>1325</v>
+      </c>
+      <c r="D91" t="s">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="B92" t="s">
+        <v>27</v>
+      </c>
+      <c r="C92" t="s">
+        <v>1336</v>
+      </c>
+      <c r="D92" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>810</v>
+      </c>
+      <c r="B93" t="s">
+        <v>39</v>
+      </c>
+      <c r="C93" t="s">
+        <v>1309</v>
+      </c>
+      <c r="D93" t="s">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="B94" t="s">
+        <v>27</v>
+      </c>
+      <c r="C94" t="s">
         <v>1334</v>
       </c>
-      <c r="D83" t="s">
-        <v>1322</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>474</v>
-      </c>
-      <c r="B84" t="s">
-        <v>20</v>
-      </c>
-      <c r="C84" t="s">
-        <v>1307</v>
-      </c>
-      <c r="D84" t="s">
-        <v>1308</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>482</v>
-      </c>
-      <c r="B85" t="s">
-        <v>39</v>
-      </c>
-      <c r="C85" t="s">
-        <v>1325</v>
-      </c>
-      <c r="D85" t="s">
-        <v>1311</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>498</v>
-      </c>
-      <c r="B86" t="s">
-        <v>10</v>
-      </c>
-      <c r="C86" t="s">
-        <v>1323</v>
-      </c>
-      <c r="D86" t="s">
-        <v>1311</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>511</v>
-      </c>
-      <c r="B87" t="s">
-        <v>27</v>
-      </c>
-      <c r="C87" t="s">
-        <v>1336</v>
-      </c>
-      <c r="D87" t="s">
-        <v>1313</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>514</v>
-      </c>
-      <c r="B88" t="s">
-        <v>10</v>
-      </c>
-      <c r="C88" t="s">
-        <v>1323</v>
-      </c>
-      <c r="D88" t="s">
-        <v>1311</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>537</v>
-      </c>
-      <c r="B89" t="s">
-        <v>20</v>
-      </c>
-      <c r="C89" t="s">
-        <v>1336</v>
-      </c>
-      <c r="D89" t="s">
-        <v>1313</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>549</v>
-      </c>
-      <c r="B90" t="s">
-        <v>27</v>
-      </c>
-      <c r="C90" t="s">
-        <v>1321</v>
-      </c>
-      <c r="D90" t="s">
-        <v>1322</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>553</v>
-      </c>
-      <c r="B91" t="s">
-        <v>39</v>
-      </c>
-      <c r="C91" t="s">
-        <v>1319</v>
-      </c>
-      <c r="D91" t="s">
-        <v>1322</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>591</v>
-      </c>
-      <c r="B92" t="s">
-        <v>27</v>
-      </c>
-      <c r="C92" t="s">
+      <c r="D94" t="s">
         <v>1310</v>
       </c>
-      <c r="D92" t="s">
-        <v>1316</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>613</v>
-      </c>
-      <c r="B93" t="s">
-        <v>10</v>
-      </c>
-      <c r="C93" t="s">
-        <v>1341</v>
-      </c>
-      <c r="D93" t="s">
-        <v>1322</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>628</v>
-      </c>
-      <c r="B94" t="s">
-        <v>10</v>
-      </c>
-      <c r="C94" t="s">
-        <v>1328</v>
-      </c>
-      <c r="D94" t="s">
-        <v>1313</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>635</v>
+    </row>
+    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>168</v>
       </c>
       <c r="B95" t="s">
         <v>27</v>
@@ -19678,141 +19674,141 @@
         <v>1323</v>
       </c>
       <c r="D95" t="s">
-        <v>1311</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>650</v>
+        <v>225</v>
       </c>
       <c r="B96" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C96" t="s">
-        <v>1321</v>
+        <v>1327</v>
       </c>
       <c r="D96" t="s">
-        <v>1322</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>657</v>
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="B97" t="s">
+        <v>27</v>
+      </c>
+      <c r="C97" t="s">
+        <v>1319</v>
+      </c>
+      <c r="D97" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
+        <v>1287</v>
+      </c>
+      <c r="B98" t="s">
+        <v>27</v>
+      </c>
+      <c r="C98" t="s">
+        <v>1319</v>
+      </c>
+      <c r="D98" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>1275</v>
+      </c>
+      <c r="B99" t="s">
+        <v>20</v>
+      </c>
+      <c r="C99" t="s">
+        <v>1325</v>
+      </c>
+      <c r="D99" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B100" t="s">
+        <v>10</v>
+      </c>
+      <c r="C100" t="s">
+        <v>1307</v>
+      </c>
+      <c r="D100" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B101" t="s">
         <v>39</v>
       </c>
-      <c r="C97" t="s">
-        <v>1309</v>
-      </c>
-      <c r="D97" t="s">
+      <c r="C101" t="s">
+        <v>1325</v>
+      </c>
+      <c r="D101" t="s">
         <v>1308</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>660</v>
-      </c>
-      <c r="B98" t="s">
-        <v>27</v>
-      </c>
-      <c r="C98" t="s">
-        <v>1323</v>
-      </c>
-      <c r="D98" t="s">
-        <v>1311</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>666</v>
-      </c>
-      <c r="B99" t="s">
+    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B102" t="s">
+        <v>27</v>
+      </c>
+      <c r="C102" t="s">
+        <v>1319</v>
+      </c>
+      <c r="D102" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B103" t="s">
         <v>39</v>
       </c>
-      <c r="C99" t="s">
-        <v>1323</v>
-      </c>
-      <c r="D99" t="s">
-        <v>1313</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>679</v>
-      </c>
-      <c r="B100" t="s">
-        <v>39</v>
-      </c>
-      <c r="C100" t="s">
-        <v>1319</v>
-      </c>
-      <c r="D100" t="s">
-        <v>1310</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>690</v>
-      </c>
-      <c r="B101" t="s">
-        <v>27</v>
-      </c>
-      <c r="C101" t="s">
-        <v>1319</v>
-      </c>
-      <c r="D101" t="s">
-        <v>1310</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>701</v>
-      </c>
-      <c r="B102" t="s">
-        <v>27</v>
-      </c>
-      <c r="C102" t="s">
-        <v>1321</v>
-      </c>
-      <c r="D102" t="s">
-        <v>1310</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>727</v>
-      </c>
-      <c r="B103" t="s">
-        <v>10</v>
-      </c>
       <c r="C103" t="s">
-        <v>1336</v>
+        <v>1325</v>
       </c>
       <c r="D103" t="s">
         <v>1311</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>730</v>
+        <v>657</v>
       </c>
       <c r="B104" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C104" t="s">
-        <v>1336</v>
+        <v>1309</v>
       </c>
       <c r="D104" t="s">
-        <v>1313</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>734</v>
+      <c r="A105" s="2" t="s">
+        <v>253</v>
       </c>
       <c r="B105" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="C105" t="s">
         <v>1307</v>
@@ -19823,586 +19819,598 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>755</v>
+        <v>53</v>
       </c>
       <c r="B106" t="s">
         <v>39</v>
       </c>
       <c r="C106" t="s">
-        <v>1321</v>
+        <v>1307</v>
       </c>
       <c r="D106" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>758</v>
+        <v>474</v>
       </c>
       <c r="B107" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="C107" t="s">
-        <v>1342</v>
+        <v>1307</v>
       </c>
       <c r="D107" t="s">
-        <v>1315</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>769</v>
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
+        <v>660</v>
       </c>
       <c r="B108" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C108" t="s">
-        <v>1336</v>
+        <v>1323</v>
       </c>
       <c r="D108" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>774</v>
+        <v>322</v>
       </c>
       <c r="B109" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C109" t="s">
-        <v>1332</v>
+        <v>1325</v>
       </c>
       <c r="D109" t="s">
-        <v>1322</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>780</v>
+        <v>1282</v>
       </c>
       <c r="B110" t="s">
         <v>27</v>
       </c>
       <c r="C110" t="s">
-        <v>1321</v>
+        <v>1325</v>
       </c>
       <c r="D110" t="s">
-        <v>1313</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>797</v>
+        <v>401</v>
       </c>
       <c r="B111" t="s">
         <v>27</v>
       </c>
       <c r="C111" t="s">
-        <v>1321</v>
+        <v>1325</v>
       </c>
       <c r="D111" t="s">
-        <v>1327</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>810</v>
+        <v>72</v>
       </c>
       <c r="B112" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="C112" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
       <c r="D112" t="s">
-        <v>1311</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>826</v>
+        <v>151</v>
       </c>
       <c r="B113" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C113" t="s">
-        <v>1309</v>
+        <v>1327</v>
       </c>
       <c r="D113" t="s">
-        <v>1311</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>833</v>
+        <v>301</v>
       </c>
       <c r="B114" t="s">
         <v>27</v>
       </c>
       <c r="C114" t="s">
-        <v>1330</v>
+        <v>1325</v>
       </c>
       <c r="D114" t="s">
-        <v>1313</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>841</v>
+        <v>98</v>
       </c>
       <c r="B115" t="s">
         <v>27</v>
       </c>
       <c r="C115" t="s">
-        <v>1332</v>
+        <v>1325</v>
       </c>
       <c r="D115" t="s">
-        <v>1310</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>848</v>
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="B116" t="s">
         <v>39</v>
       </c>
       <c r="C116" t="s">
-        <v>1336</v>
+        <v>1323</v>
       </c>
       <c r="D116" t="s">
         <v>1311</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>851</v>
+    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="B117" t="s">
         <v>27</v>
       </c>
       <c r="C117" t="s">
-        <v>1325</v>
+        <v>1319</v>
       </c>
       <c r="D117" t="s">
-        <v>1308</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>854</v>
+        <v>331</v>
       </c>
       <c r="B118" t="s">
         <v>10</v>
       </c>
       <c r="C118" t="s">
-        <v>1319</v>
+        <v>1307</v>
       </c>
       <c r="D118" t="s">
-        <v>1313</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>863</v>
+        <v>129</v>
       </c>
       <c r="B119" t="s">
         <v>20</v>
       </c>
       <c r="C119" t="s">
-        <v>1319</v>
+        <v>1327</v>
       </c>
       <c r="D119" t="s">
-        <v>1322</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>870</v>
+        <v>734</v>
       </c>
       <c r="B120" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C120" t="s">
-        <v>1319</v>
+        <v>1307</v>
       </c>
       <c r="D120" t="s">
-        <v>1313</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>883</v>
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
+        <v>635</v>
       </c>
       <c r="B121" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="C121" t="s">
-        <v>1336</v>
+        <v>1323</v>
       </c>
       <c r="D121" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>888</v>
+        <v>1217</v>
       </c>
       <c r="B122" t="s">
         <v>10</v>
       </c>
       <c r="C122" t="s">
-        <v>1332</v>
+        <v>1307</v>
       </c>
       <c r="D122" t="s">
-        <v>1322</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>897</v>
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B123" t="s">
+        <v>10</v>
       </c>
       <c r="C123" t="s">
-        <v>1309</v>
+        <v>1323</v>
       </c>
       <c r="D123" t="s">
-        <v>1309</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>903</v>
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
+        <v>436</v>
       </c>
       <c r="B124" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C124" t="s">
-        <v>1336</v>
+        <v>1323</v>
       </c>
       <c r="D124" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>909</v>
+        <v>851</v>
       </c>
       <c r="B125" t="s">
+        <v>27</v>
+      </c>
+      <c r="C125" t="s">
+        <v>1325</v>
+      </c>
+      <c r="D125" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B126" t="s">
         <v>39</v>
-      </c>
-      <c r="C125" t="s">
-        <v>1330</v>
-      </c>
-      <c r="D125" t="s">
-        <v>1313</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>912</v>
-      </c>
-      <c r="B126" t="s">
-        <v>20</v>
       </c>
       <c r="C126" t="s">
         <v>1323</v>
       </c>
       <c r="D126" t="s">
-        <v>1322</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>917</v>
+        <v>11</v>
       </c>
       <c r="B127" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C127" t="s">
-        <v>1336</v>
+        <v>1307</v>
       </c>
       <c r="D127" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B128" t="s">
+        <v>10</v>
+      </c>
+      <c r="C128" t="s">
+        <v>1312</v>
+      </c>
+      <c r="D128" t="s">
         <v>1313</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>941</v>
-      </c>
-      <c r="B128" t="s">
-        <v>20</v>
-      </c>
-      <c r="C128" t="s">
-        <v>1321</v>
-      </c>
-      <c r="D128" t="s">
-        <v>1322</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>867</v>
+    <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="B129" t="s">
+        <v>10</v>
       </c>
       <c r="C129" t="s">
-        <v>1336</v>
+        <v>1323</v>
       </c>
       <c r="D129" t="s">
-        <v>1310</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>959</v>
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
+        <v>498</v>
       </c>
       <c r="B130" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C130" t="s">
-        <v>1332</v>
+        <v>1323</v>
       </c>
       <c r="D130" t="s">
-        <v>1310</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>962</v>
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="2" t="s">
+        <v>204</v>
       </c>
       <c r="B131" t="s">
         <v>39</v>
       </c>
       <c r="C131" t="s">
-        <v>1309</v>
+        <v>1323</v>
       </c>
       <c r="D131" t="s">
-        <v>1313</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>975</v>
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B132" t="s">
+        <v>10</v>
       </c>
       <c r="C132" t="s">
-        <v>1309</v>
+        <v>1319</v>
       </c>
       <c r="D132" t="s">
-        <v>1309</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>984</v>
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="B133" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C133" t="s">
-        <v>1336</v>
+        <v>1314</v>
       </c>
       <c r="D133" t="s">
-        <v>1313</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>987</v>
+        <v>758</v>
       </c>
       <c r="B134" t="s">
         <v>39</v>
       </c>
       <c r="C134" t="s">
-        <v>1321</v>
+        <v>1342</v>
       </c>
       <c r="D134" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>337</v>
+      </c>
+      <c r="B135" t="s">
+        <v>27</v>
+      </c>
+      <c r="C135" t="s">
+        <v>1337</v>
+      </c>
+      <c r="D135" t="s">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>21</v>
+      </c>
+      <c r="B136" t="s">
+        <v>20</v>
+      </c>
+      <c r="C136" t="s">
         <v>1310</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+      <c r="D136" t="s">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="B137" t="s">
+        <v>27</v>
+      </c>
+      <c r="C137" t="s">
+        <v>1338</v>
+      </c>
+      <c r="D137" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
         <v>1048</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B138" t="s">
         <v>39</v>
       </c>
-      <c r="C135" t="s">
+      <c r="C138" t="s">
         <v>1309</v>
       </c>
-      <c r="D135" t="s">
+      <c r="D138" t="s">
         <v>1310</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>1091</v>
-      </c>
-      <c r="B136" t="s">
-        <v>10</v>
-      </c>
-      <c r="C136" t="s">
-        <v>1307</v>
-      </c>
-      <c r="D136" t="s">
-        <v>1313</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>1100</v>
-      </c>
-      <c r="B137" t="s">
-        <v>10</v>
-      </c>
-      <c r="C137" t="s">
-        <v>1323</v>
-      </c>
-      <c r="D137" t="s">
-        <v>1311</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>1111</v>
-      </c>
-      <c r="B138" t="s">
-        <v>20</v>
-      </c>
-      <c r="C138" t="s">
-        <v>1325</v>
-      </c>
-      <c r="D138" t="s">
-        <v>1313</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>1118</v>
+        <v>155</v>
       </c>
       <c r="B139" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="C139" t="s">
-        <v>1325</v>
+        <v>1329</v>
       </c>
       <c r="D139" t="s">
-        <v>1313</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>1145</v>
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
+        <v>727</v>
       </c>
       <c r="B140" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C140" t="s">
-        <v>1321</v>
+        <v>1336</v>
       </c>
       <c r="D140" t="s">
-        <v>1310</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>1157</v>
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
+        <v>1222</v>
       </c>
       <c r="B141" t="s">
         <v>39</v>
       </c>
       <c r="C141" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="D141" t="s">
-        <v>1311</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>1192</v>
+        <v>284</v>
       </c>
       <c r="B142" t="s">
+        <v>10</v>
+      </c>
+      <c r="C142" t="s">
+        <v>1310</v>
+      </c>
+      <c r="D142" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B143" t="s">
+        <v>20</v>
+      </c>
+      <c r="C143" t="s">
+        <v>1310</v>
+      </c>
+      <c r="D143" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>40</v>
+      </c>
+      <c r="B144" t="s">
         <v>39</v>
       </c>
-      <c r="C142" t="s">
-        <v>1309</v>
-      </c>
-      <c r="D142" t="s">
-        <v>1308</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>1199</v>
-      </c>
-      <c r="B143" t="s">
-        <v>27</v>
-      </c>
-      <c r="C143" t="s">
-        <v>1319</v>
-      </c>
-      <c r="D143" t="s">
-        <v>1327</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>1217</v>
-      </c>
-      <c r="B144" t="s">
-        <v>10</v>
-      </c>
       <c r="C144" t="s">
-        <v>1307</v>
+        <v>1310</v>
       </c>
       <c r="D144" t="s">
-        <v>1311</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>1222</v>
+        <v>361</v>
       </c>
       <c r="B145" t="s">
         <v>39</v>
       </c>
       <c r="C145" t="s">
-        <v>1321</v>
+        <v>1327</v>
       </c>
       <c r="D145" t="s">
-        <v>1327</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>1225</v>
+        <v>163</v>
+      </c>
+      <c r="B146" t="s">
+        <v>10</v>
       </c>
       <c r="C146" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="D146" t="s">
-        <v>1309</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>1228</v>
+        <v>1236</v>
       </c>
       <c r="B147" t="s">
-        <v>673</v>
+        <v>10</v>
       </c>
       <c r="C147" t="s">
         <v>1310</v>
       </c>
       <c r="D147" t="s">
-        <v>1308</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>1236</v>
+        <v>211</v>
       </c>
       <c r="B148" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C148" t="s">
         <v>1310</v>
@@ -20411,56 +20419,65 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>1241</v>
+        <v>267</v>
+      </c>
+      <c r="B149" t="s">
+        <v>27</v>
       </c>
       <c r="C149" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="D149" t="s">
-        <v>1309</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>1256</v>
+        <v>462</v>
+      </c>
+      <c r="B150" t="s">
+        <v>39</v>
       </c>
       <c r="C150" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="D150" t="s">
-        <v>1309</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>1259</v>
+        <v>591</v>
       </c>
       <c r="B151" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C151" t="s">
-        <v>1322</v>
+        <v>1310</v>
       </c>
       <c r="D151" t="s">
         <v>1316</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>1263</v>
+    <row r="152" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B152" t="s">
+        <v>27</v>
       </c>
       <c r="C152" t="s">
-        <v>1309</v>
+        <v>1319</v>
       </c>
       <c r="D152" t="s">
-        <v>1309</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>1268</v>
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="C153" t="s">
         <v>1309</v>
@@ -20469,51 +20486,48 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>1275</v>
+    <row r="154" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="B154" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C154" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="D154" t="s">
-        <v>1308</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>1282</v>
+        <v>1192</v>
       </c>
       <c r="B155" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C155" t="s">
-        <v>1325</v>
+        <v>1309</v>
       </c>
       <c r="D155" t="s">
         <v>1308</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>1287</v>
-      </c>
-      <c r="B156" t="s">
-        <v>27</v>
+    <row r="156" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="2" t="s">
+        <v>867</v>
       </c>
       <c r="C156" t="s">
-        <v>1319</v>
+        <v>1336</v>
       </c>
       <c r="D156" t="s">
-        <v>1313</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>1294</v>
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="2" t="s">
+        <v>1199</v>
       </c>
       <c r="B157" t="s">
         <v>27</v>
@@ -20522,25 +20536,40 @@
         <v>1319</v>
       </c>
       <c r="D157" t="s">
-        <v>1313</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>1299</v>
+        <v>194</v>
       </c>
       <c r="B158" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C158" t="s">
-        <v>1310</v>
+        <v>1325</v>
       </c>
       <c r="D158" t="s">
-        <v>1316</v>
+        <v>1311</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D158">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="10"/>
+        <filter val="6,7,8,9"/>
+        <filter val="7,9"/>
+        <filter val="8,9"/>
+        <filter val="9"/>
+      </filters>
+    </filterColumn>
+    <sortState ref="A2:D158">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -20551,6 +20580,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -20791,9 +20826,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
actualizaciones de excel varios
</commit_message>
<xml_diff>
--- a/excels/niveles_unificados1.3.xlsx
+++ b/excels/niveles_unificados1.3.xlsx
@@ -18374,9 +18374,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:D158"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A158" sqref="A158"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18554,7 +18552,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>1118</v>
       </c>
@@ -18940,7 +18938,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>482</v>
       </c>
@@ -18954,7 +18952,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>1091</v>
       </c>
@@ -18968,7 +18966,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>389</v>
       </c>
@@ -19178,7 +19176,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>236</v>
       </c>
@@ -19304,7 +19302,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>1111</v>
       </c>
@@ -19607,7 +19605,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>183</v>
       </c>
@@ -19719,7 +19717,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>1275</v>
       </c>
@@ -19733,7 +19731,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>275</v>
       </c>
@@ -19747,7 +19745,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>348</v>
       </c>
@@ -19775,7 +19773,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>298</v>
       </c>
@@ -19803,7 +19801,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>253</v>
       </c>
@@ -19817,7 +19815,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>53</v>
       </c>
@@ -19831,7 +19829,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>474</v>
       </c>
@@ -19859,7 +19857,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>322</v>
       </c>
@@ -19873,7 +19871,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>1282</v>
       </c>
@@ -19901,7 +19899,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>72</v>
       </c>
@@ -19916,7 +19914,7 @@
       </c>
     </row>
     <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+      <c r="A113" s="2" t="s">
         <v>151</v>
       </c>
       <c r="B113" t="s">
@@ -19929,7 +19927,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>301</v>
       </c>
@@ -19943,7 +19941,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>98</v>
       </c>
@@ -19985,7 +19983,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>331</v>
       </c>
@@ -20000,7 +19998,7 @@
       </c>
     </row>
     <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+      <c r="A119" s="2" t="s">
         <v>129</v>
       </c>
       <c r="B119" t="s">
@@ -20013,7 +20011,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>734</v>
       </c>
@@ -20041,7 +20039,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>1217</v>
       </c>
@@ -20083,7 +20081,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>851</v>
       </c>
@@ -20111,7 +20109,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>11</v>
       </c>
@@ -20279,7 +20277,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>155</v>
       </c>
@@ -20539,7 +20537,7 @@
         <v>1327</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>194</v>
       </c>
@@ -20555,13 +20553,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:D158">
-    <filterColumn colId="2">
+    <filterColumn colId="0">
       <filters>
-        <filter val="10"/>
-        <filter val="6,7,8,9"/>
-        <filter val="7,9"/>
-        <filter val="8,9"/>
-        <filter val="9"/>
+        <filter val="Jefe De Mantención"/>
       </filters>
     </filterColumn>
     <sortState ref="A2:D158">

</xml_diff>

<commit_message>
se estandarizo los niveles y cargaron a la base, se cargaron en el dashboard y ya se puede filtrar por niveles
</commit_message>
<xml_diff>
--- a/excels/niveles_unificados1.3.xlsx
+++ b/excels/niveles_unificados1.3.xlsx
@@ -18371,10 +18371,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:D158"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18398,7 +18399,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>848</v>
       </c>
@@ -18412,7 +18413,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>188</v>
       </c>
@@ -18426,7 +18427,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>797</v>
       </c>
@@ -18440,7 +18441,7 @@
         <v>1327</v>
       </c>
     </row>
-    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>158</v>
       </c>
@@ -18454,7 +18455,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>888</v>
       </c>
@@ -18468,7 +18469,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>962</v>
       </c>
@@ -18482,7 +18483,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>903</v>
       </c>
@@ -18496,7 +18497,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>613</v>
       </c>
@@ -18510,7 +18511,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>396</v>
       </c>
@@ -18524,7 +18525,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>256</v>
       </c>
@@ -18538,7 +18539,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>469</v>
       </c>
@@ -18552,7 +18553,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>1118</v>
       </c>
@@ -18566,7 +18567,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>883</v>
       </c>
@@ -18580,7 +18581,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>841</v>
       </c>
@@ -18594,7 +18595,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>371</v>
       </c>
@@ -18608,7 +18609,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>909</v>
       </c>
@@ -18622,7 +18623,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>553</v>
       </c>
@@ -18636,7 +18637,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>959</v>
       </c>
@@ -18650,7 +18651,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>191</v>
       </c>
@@ -18664,7 +18665,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>897</v>
       </c>
@@ -18675,7 +18676,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>917</v>
       </c>
@@ -18689,7 +18690,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>171</v>
       </c>
@@ -18703,7 +18704,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>58</v>
       </c>
@@ -18714,7 +18715,7 @@
         <v>1307</v>
       </c>
     </row>
-    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>214</v>
       </c>
@@ -18728,7 +18729,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>755</v>
       </c>
@@ -18742,7 +18743,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>239</v>
       </c>
@@ -18756,7 +18757,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>231</v>
       </c>
@@ -18770,7 +18771,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>75</v>
       </c>
@@ -18784,7 +18785,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>987</v>
       </c>
@@ -18798,7 +18799,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>701</v>
       </c>
@@ -18812,7 +18813,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>1145</v>
       </c>
@@ -18826,7 +18827,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>45</v>
       </c>
@@ -18840,7 +18841,7 @@
         <v>1307</v>
       </c>
     </row>
-    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>679</v>
       </c>
@@ -18854,7 +18855,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>826</v>
       </c>
@@ -18868,7 +18869,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>177</v>
       </c>
@@ -18882,7 +18883,7 @@
         <v>1307</v>
       </c>
     </row>
-    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>248</v>
       </c>
@@ -18896,7 +18897,7 @@
         <v>1327</v>
       </c>
     </row>
-    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>259</v>
       </c>
@@ -18910,7 +18911,7 @@
         <v>1327</v>
       </c>
     </row>
-    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>91</v>
       </c>
@@ -18924,7 +18925,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>666</v>
       </c>
@@ -18938,7 +18939,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>482</v>
       </c>
@@ -18952,7 +18953,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>1091</v>
       </c>
@@ -18966,7 +18967,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>389</v>
       </c>
@@ -18980,7 +18981,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>272</v>
       </c>
@@ -18994,7 +18995,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>1228</v>
       </c>
@@ -19008,7 +19009,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>774</v>
       </c>
@@ -19022,7 +19023,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>136</v>
       </c>
@@ -19036,7 +19037,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>650</v>
       </c>
@@ -19050,7 +19051,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>262</v>
       </c>
@@ -19064,7 +19065,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>424</v>
       </c>
@@ -19078,7 +19079,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>78</v>
       </c>
@@ -19092,7 +19093,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>730</v>
       </c>
@@ -19106,7 +19107,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>780</v>
       </c>
@@ -19120,7 +19121,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>870</v>
       </c>
@@ -19134,7 +19135,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>180</v>
       </c>
@@ -19148,7 +19149,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>549</v>
       </c>
@@ -19162,7 +19163,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>412</v>
       </c>
@@ -19176,7 +19177,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>236</v>
       </c>
@@ -19190,7 +19191,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>295</v>
       </c>
@@ -19204,7 +19205,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>378</v>
       </c>
@@ -19218,7 +19219,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>94</v>
       </c>
@@ -19232,7 +19233,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>280</v>
       </c>
@@ -19246,7 +19247,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>984</v>
       </c>
@@ -19260,7 +19261,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>292</v>
       </c>
@@ -19274,7 +19275,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>769</v>
       </c>
@@ -19288,7 +19289,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>364</v>
       </c>
@@ -19302,7 +19303,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>1111</v>
       </c>
@@ -19316,7 +19317,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>537</v>
       </c>
@@ -19330,7 +19331,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>421</v>
       </c>
@@ -19344,7 +19345,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>628</v>
       </c>
@@ -19358,7 +19359,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>854</v>
       </c>
@@ -19372,7 +19373,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>833</v>
       </c>
@@ -19386,7 +19387,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>220</v>
       </c>
@@ -19400,7 +19401,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>17</v>
       </c>
@@ -19411,7 +19412,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>14</v>
       </c>
@@ -19422,7 +19423,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>1241</v>
       </c>
@@ -19433,7 +19434,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>1256</v>
       </c>
@@ -19444,7 +19445,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>228</v>
       </c>
@@ -19455,7 +19456,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>1225</v>
       </c>
@@ -19466,7 +19467,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>112</v>
       </c>
@@ -19477,7 +19478,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>1268</v>
       </c>
@@ -19488,7 +19489,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>107</v>
       </c>
@@ -19499,7 +19500,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>1259</v>
       </c>
@@ -19513,7 +19514,7 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>1263</v>
       </c>
@@ -19524,7 +19525,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>941</v>
       </c>
@@ -19538,7 +19539,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>863</v>
       </c>
@@ -19552,7 +19553,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>912</v>
       </c>
@@ -19566,7 +19567,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>132</v>
       </c>
@@ -19580,7 +19581,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>975</v>
       </c>
@@ -19591,7 +19592,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>690</v>
       </c>
@@ -19605,7 +19606,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>183</v>
       </c>
@@ -19619,7 +19620,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>511</v>
       </c>
@@ -19633,7 +19634,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>810</v>
       </c>
@@ -19647,7 +19648,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="94" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>447</v>
       </c>
@@ -19661,7 +19662,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>168</v>
       </c>
@@ -19675,7 +19676,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>225</v>
       </c>
@@ -19689,7 +19690,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>124</v>
       </c>
@@ -19703,7 +19704,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>1287</v>
       </c>
@@ -19717,7 +19718,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>1275</v>
       </c>
@@ -19731,7 +19732,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>275</v>
       </c>
@@ -19745,7 +19746,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>348</v>
       </c>
@@ -19759,7 +19760,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>1294</v>
       </c>
@@ -19773,7 +19774,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>298</v>
       </c>
@@ -19787,7 +19788,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="104" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>657</v>
       </c>
@@ -19801,7 +19802,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>253</v>
       </c>
@@ -19815,7 +19816,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="106" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>53</v>
       </c>
@@ -19829,7 +19830,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>474</v>
       </c>
@@ -19843,7 +19844,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="108" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>660</v>
       </c>
@@ -19857,7 +19858,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="109" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>322</v>
       </c>
@@ -19871,7 +19872,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>1282</v>
       </c>
@@ -19899,7 +19900,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>72</v>
       </c>
@@ -19913,7 +19914,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>151</v>
       </c>
@@ -19927,7 +19928,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>301</v>
       </c>
@@ -19941,7 +19942,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>98</v>
       </c>
@@ -19955,7 +19956,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>88</v>
       </c>
@@ -19969,7 +19970,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>65</v>
       </c>
@@ -19983,7 +19984,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="118" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>331</v>
       </c>
@@ -19997,7 +19998,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>129</v>
       </c>
@@ -20011,7 +20012,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>734</v>
       </c>
@@ -20025,7 +20026,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>635</v>
       </c>
@@ -20039,7 +20040,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>1217</v>
       </c>
@@ -20053,7 +20054,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="123" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>1100</v>
       </c>
@@ -20067,7 +20068,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="124" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>436</v>
       </c>
@@ -20081,7 +20082,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="125" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>851</v>
       </c>
@@ -20095,7 +20096,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="126" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>1157</v>
       </c>
@@ -20109,7 +20110,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>11</v>
       </c>
@@ -20123,7 +20124,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>24</v>
       </c>
@@ -20137,7 +20138,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>514</v>
       </c>
@@ -20151,7 +20152,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>498</v>
       </c>
@@ -20165,7 +20166,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>204</v>
       </c>
@@ -20179,7 +20180,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="132" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>217</v>
       </c>
@@ -20193,7 +20194,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>28</v>
       </c>
@@ -20207,7 +20208,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>758</v>
       </c>
@@ -20221,7 +20222,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="135" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>337</v>
       </c>
@@ -20235,7 +20236,7 @@
         <v>1307</v>
       </c>
     </row>
-    <row r="136" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>21</v>
       </c>
@@ -20249,7 +20250,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="137" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>343</v>
       </c>
@@ -20263,7 +20264,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="138" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>1048</v>
       </c>
@@ -20277,7 +20278,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="139" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>155</v>
       </c>
@@ -20291,7 +20292,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="140" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>727</v>
       </c>
@@ -20305,7 +20306,7 @@
         <v>1311</v>
       </c>
     </row>
-    <row r="141" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>1222</v>
       </c>
@@ -20319,7 +20320,7 @@
         <v>1327</v>
       </c>
     </row>
-    <row r="142" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>284</v>
       </c>
@@ -20333,7 +20334,7 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="143" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>1299</v>
       </c>
@@ -20347,7 +20348,7 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="144" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>40</v>
       </c>
@@ -20361,7 +20362,7 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="145" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>361</v>
       </c>
@@ -20375,7 +20376,7 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="146" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>163</v>
       </c>
@@ -20389,7 +20390,7 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="147" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>1236</v>
       </c>
@@ -20403,7 +20404,7 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="148" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>211</v>
       </c>
@@ -20417,7 +20418,7 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="149" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>267</v>
       </c>
@@ -20431,7 +20432,7 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="150" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>462</v>
       </c>
@@ -20445,7 +20446,7 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="151" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>591</v>
       </c>
@@ -20459,7 +20460,7 @@
         <v>1316</v>
       </c>
     </row>
-    <row r="152" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>83</v>
       </c>
@@ -20473,7 +20474,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="153" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>317</v>
       </c>
@@ -20484,7 +20485,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="154" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>117</v>
       </c>
@@ -20498,7 +20499,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="155" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>1192</v>
       </c>
@@ -20512,7 +20513,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="156" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>867</v>
       </c>
@@ -20523,7 +20524,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="157" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>1199</v>
       </c>
@@ -20537,7 +20538,7 @@
         <v>1327</v>
       </c>
     </row>
-    <row r="158" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>194</v>
       </c>
@@ -20553,11 +20554,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:D158">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Jefe De Mantención"/>
-      </filters>
-    </filterColumn>
     <sortState ref="A2:D158">
       <sortCondition ref="A1"/>
     </sortState>

</xml_diff>